<commit_message>
add NH4 rerun results
</commit_message>
<xml_diff>
--- a/FCM/Osnat_CC1A3_N analysis.xlsx
+++ b/FCM/Osnat_CC1A3_N analysis.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\CC1A3\FCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B174685A-3760-46B4-A8F3-CEB0C888E399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E72C073-C8B1-4ABB-B53D-DF4FBDBC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="7" xr2:uid="{B9BD0F45-4C1D-413E-AD5C-7BE548D4C230}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{B9BD0F45-4C1D-413E-AD5C-7BE548D4C230}"/>
   </bookViews>
   <sheets>
     <sheet name="N budget" sheetId="15" r:id="rId1"/>
-    <sheet name="NO3 06112023" sheetId="14" r:id="rId2"/>
-    <sheet name="NH4 06112023" sheetId="13" r:id="rId3"/>
-    <sheet name="samples" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="231106_Osnat_NH4.run RRR" sheetId="5" r:id="rId6"/>
-    <sheet name="231106_Osnat_NH4 contR1 RRR" sheetId="8" r:id="rId7"/>
-    <sheet name="DON2DIN rate" sheetId="11" r:id="rId8"/>
-    <sheet name="231106_Osnat_NO3R1 RRR" sheetId="12" r:id="rId9"/>
+    <sheet name="NH4 rerun" sheetId="16" r:id="rId2"/>
+    <sheet name="NO3 06112023" sheetId="14" r:id="rId3"/>
+    <sheet name="NH4 06112023" sheetId="13" r:id="rId4"/>
+    <sheet name="samples" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="231106_Osnat_NH4.run RRR" sheetId="5" r:id="rId7"/>
+    <sheet name="231106_Osnat_NH4 contR1 RRR" sheetId="8" r:id="rId8"/>
+    <sheet name="DON2DIN rate" sheetId="11" r:id="rId9"/>
+    <sheet name="231106_Osnat_NO3R1 RRR" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="154">
   <si>
     <t>P1A</t>
   </si>
@@ -612,6 +613,30 @@
   <si>
     <t>log(DON)</t>
   </si>
+  <si>
+    <t>The values were 0.326 and 0.543 uM for the P99 and A5A samples, respectively, which means 163 and 271 uM in the original samples. </t>
+  </si>
+  <si>
+    <t>P99</t>
+  </si>
+  <si>
+    <t>previous run measured (uM)</t>
+  </si>
+  <si>
+    <t>rerun measured (uM NH4)</t>
+  </si>
+  <si>
+    <t>retrun dilution</t>
+  </si>
+  <si>
+    <t>retrun final (uM NH4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previous run dilution </t>
+  </si>
+  <si>
+    <t>previous run final (uM)</t>
+  </si>
 </sst>
 </file>
 
@@ -750,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -814,12 +839,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6831,9 +6942,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6871,7 +6982,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6977,7 +7088,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7119,7 +7230,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8819,7 +8930,1418 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD832222-DA15-455F-8288-674CD472E732}">
+  <dimension ref="A1:K60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="K6">
+        <v>44429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7">
+        <v>7815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>7049</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>62700</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>68132</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>64125</v>
+      </c>
+      <c r="H16">
+        <v>1.27</v>
+      </c>
+      <c r="I16">
+        <f>(G16-$K$7)/$K$6</f>
+        <v>1.2674154268608342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>49144</v>
+      </c>
+      <c r="H17">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I32" si="0">(G17-$K$7)/$K$6</f>
+        <v>0.93022575344932368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>35394</v>
+      </c>
+      <c r="H18">
+        <v>0.63</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.62074320826487206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>23240</v>
+      </c>
+      <c r="H19">
+        <v>0.316</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.34718314614328477</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>6991</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>-1.8546444889599136E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>106336</v>
+      </c>
+      <c r="H21">
+        <v>2.3279999999999998</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>2.2174930788448988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>107802</v>
+      </c>
+      <c r="H22">
+        <v>2.3811</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>2.250489545116928</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>82820</v>
+      </c>
+      <c r="H23">
+        <v>1.7745</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>1.6881991492043484</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>54544</v>
+      </c>
+      <c r="H24">
+        <v>1.1053999999999999</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>1.0517679893763083</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>76885</v>
+      </c>
+      <c r="H25">
+        <v>1.6415</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>1.5546152287920052</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>66680</v>
+      </c>
+      <c r="H26">
+        <v>1.3872</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>1.3249229107114722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>62657</v>
+      </c>
+      <c r="H27">
+        <v>1.2826</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>1.2343739449458686</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>36768</v>
+      </c>
+      <c r="H28">
+        <v>0.68540000000000001</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0.65166895496184929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>31754</v>
+      </c>
+      <c r="H29">
+        <v>0.57720000000000005</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.53881473812149727</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>35000</v>
+      </c>
+      <c r="H30">
+        <v>0.6694</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.61187512660649579</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>32293</v>
+      </c>
+      <c r="H31">
+        <v>0.57140000000000002</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0.55094645389272767</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>50620</v>
+      </c>
+      <c r="H32">
+        <v>0.9879</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0.96344729793603279</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>7049</v>
+      </c>
+      <c r="H41">
+        <v>-4.6300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>62706</v>
+      </c>
+      <c r="H42">
+        <v>1.2432000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>68144</v>
+      </c>
+      <c r="H43">
+        <v>1.3692</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>64144</v>
+      </c>
+      <c r="H44">
+        <v>1.2765</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>49169</v>
+      </c>
+      <c r="H45">
+        <v>0.92959999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>35427</v>
+      </c>
+      <c r="H46">
+        <v>0.61119999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>23279</v>
+      </c>
+      <c r="H47">
+        <v>0.32969999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>7049</v>
+      </c>
+      <c r="H48">
+        <v>-4.6300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>106402</v>
+      </c>
+      <c r="H49">
+        <v>2.2555000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>107875</v>
+      </c>
+      <c r="H50">
+        <v>2.2896999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>82900</v>
+      </c>
+      <c r="H51">
+        <v>1.7110000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>54630</v>
+      </c>
+      <c r="H52">
+        <v>1.0561</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>76978</v>
+      </c>
+      <c r="H53">
+        <v>1.5738000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>66780</v>
+      </c>
+      <c r="H54">
+        <v>1.3375999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>62764</v>
+      </c>
+      <c r="H55">
+        <v>1.2444999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>36881</v>
+      </c>
+      <c r="H56">
+        <v>0.64490000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>31874</v>
+      </c>
+      <c r="H57">
+        <v>0.52890000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>17</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>35126</v>
+      </c>
+      <c r="H58">
+        <v>0.60419999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>32427</v>
+      </c>
+      <c r="H59">
+        <v>0.54169999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>50760</v>
+      </c>
+      <c r="H60">
+        <v>0.96640000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7DF78F-93CC-4C78-98B4-1C8663CCD867}">
+  <dimension ref="A2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="7" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="45">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="28">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="C6" s="28">
+        <v>500</v>
+      </c>
+      <c r="D6" s="28">
+        <f>B6*C6</f>
+        <v>163</v>
+      </c>
+      <c r="E6" s="29">
+        <v>1.4699026071910759</v>
+      </c>
+      <c r="F6" s="28">
+        <v>100</v>
+      </c>
+      <c r="G6" s="30">
+        <f t="shared" ref="G6" si="0">E6*100</f>
+        <v>146.9902607191076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="C7" s="28">
+        <v>500</v>
+      </c>
+      <c r="D7" s="28">
+        <f>B7*C7</f>
+        <v>271.5</v>
+      </c>
+      <c r="E7" s="29">
+        <v>2.7525776979643197</v>
+      </c>
+      <c r="F7" s="30">
+        <v>100</v>
+      </c>
+      <c r="G7" s="30">
+        <f t="shared" ref="G7" si="1">E7*100</f>
+        <v>275.25776979643194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10E03E2-079B-4BA4-A3C9-994DFF051B89}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -9088,12 +10610,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D0E95B-CCEE-458C-A4BC-7AB1E8727653}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10290,10 +11812,10 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D52">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0.517</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0.129</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10302,7 +11824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0EBF05-3BB1-4FFD-AA04-244B0A8D102B}">
   <dimension ref="A1:E132"/>
   <sheetViews>
@@ -11264,7 +12786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A80636-E6B2-465F-82CF-957E30DF8F39}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -11334,7 +12856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83FB972-B64F-451D-BD00-A19A23087774}">
   <dimension ref="A1:K96"/>
   <sheetViews>
@@ -13671,7 +15193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D460E32-3447-4944-955F-FB3B778FB3E9}">
   <dimension ref="A1:K72"/>
   <sheetViews>
@@ -15313,11 +16835,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587D7273-4071-4F27-B14B-00717A86561F}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -15724,1323 +17246,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD832222-DA15-455F-8288-674CD472E732}">
-  <dimension ref="A1:K60"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="K6">
-        <v>44429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7">
-        <v>7815</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>7049</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>62700</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>68132</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>64125</v>
-      </c>
-      <c r="H16">
-        <v>1.27</v>
-      </c>
-      <c r="I16">
-        <f>(G16-$K$7)/$K$6</f>
-        <v>1.2674154268608342</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>49144</v>
-      </c>
-      <c r="H17">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="I17">
-        <f t="shared" ref="I17:I32" si="0">(G17-$K$7)/$K$6</f>
-        <v>0.93022575344932368</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>35394</v>
-      </c>
-      <c r="H18">
-        <v>0.63</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0.62074320826487206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>23240</v>
-      </c>
-      <c r="H19">
-        <v>0.316</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0.34718314614328477</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>6991</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>-1.8546444889599136E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>106336</v>
-      </c>
-      <c r="H21">
-        <v>2.3279999999999998</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>2.2174930788448988</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>107802</v>
-      </c>
-      <c r="H22">
-        <v>2.3811</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>2.250489545116928</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>82820</v>
-      </c>
-      <c r="H23">
-        <v>1.7745</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>1.6881991492043484</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24">
-        <v>11</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>54544</v>
-      </c>
-      <c r="H24">
-        <v>1.1053999999999999</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>1.0517679893763083</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>76885</v>
-      </c>
-      <c r="H25">
-        <v>1.6415</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>1.5546152287920052</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>66680</v>
-      </c>
-      <c r="H26">
-        <v>1.3872</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>1.3249229107114722</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>62657</v>
-      </c>
-      <c r="H27">
-        <v>1.2826</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>1.2343739449458686</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>36768</v>
-      </c>
-      <c r="H28">
-        <v>0.68540000000000001</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0.65166895496184929</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29">
-        <v>16</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>31754</v>
-      </c>
-      <c r="H29">
-        <v>0.57720000000000005</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0.53881473812149727</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>35000</v>
-      </c>
-      <c r="H30">
-        <v>0.6694</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0.61187512660649579</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31">
-        <v>18</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>32293</v>
-      </c>
-      <c r="H31">
-        <v>0.57140000000000002</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>0.55094645389272767</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>50620</v>
-      </c>
-      <c r="H32">
-        <v>0.9879</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>0.96344729793603279</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" t="s">
-        <v>81</v>
-      </c>
-      <c r="H36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" t="s">
-        <v>74</v>
-      </c>
-      <c r="H38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H39" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>7049</v>
-      </c>
-      <c r="H41">
-        <v>-4.6300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>62706</v>
-      </c>
-      <c r="H42">
-        <v>1.2432000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43">
-        <v>2</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>68144</v>
-      </c>
-      <c r="H43">
-        <v>1.3692</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>64144</v>
-      </c>
-      <c r="H44">
-        <v>1.2765</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45">
-        <v>4</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>49169</v>
-      </c>
-      <c r="H45">
-        <v>0.92959999999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>35427</v>
-      </c>
-      <c r="H46">
-        <v>0.61119999999999997</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>23279</v>
-      </c>
-      <c r="H47">
-        <v>0.32969999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48">
-        <v>7</v>
-      </c>
-      <c r="B48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>7049</v>
-      </c>
-      <c r="H48">
-        <v>-4.6300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49">
-        <v>8</v>
-      </c>
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>106402</v>
-      </c>
-      <c r="H49">
-        <v>2.2555000000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50">
-        <v>9</v>
-      </c>
-      <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>107875</v>
-      </c>
-      <c r="H50">
-        <v>2.2896999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51">
-        <v>10</v>
-      </c>
-      <c r="B51" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" t="s">
-        <v>98</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>82900</v>
-      </c>
-      <c r="H51">
-        <v>1.7110000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52">
-        <v>11</v>
-      </c>
-      <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" t="s">
-        <v>98</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>54630</v>
-      </c>
-      <c r="H52">
-        <v>1.0561</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53">
-        <v>12</v>
-      </c>
-      <c r="B53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" t="s">
-        <v>98</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>76978</v>
-      </c>
-      <c r="H53">
-        <v>1.5738000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>66780</v>
-      </c>
-      <c r="H54">
-        <v>1.3375999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" t="s">
-        <v>98</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>62764</v>
-      </c>
-      <c r="H55">
-        <v>1.2444999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56">
-        <v>15</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>36881</v>
-      </c>
-      <c r="H56">
-        <v>0.64490000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57">
-        <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>31874</v>
-      </c>
-      <c r="H57">
-        <v>0.52890000000000004</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58">
-        <v>17</v>
-      </c>
-      <c r="B58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>35126</v>
-      </c>
-      <c r="H58">
-        <v>0.60419999999999996</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>32427</v>
-      </c>
-      <c r="H59">
-        <v>0.54169999999999996</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60">
-        <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>50760</v>
-      </c>
-      <c r="H60">
-        <v>0.96640000000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>